<commit_message>
adding a exact date in Horario_Tutor table
</commit_message>
<xml_diff>
--- a/20240914 - Data.xlsx
+++ b/20240914 - Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GitHub\tutoring-school\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA43C957-E702-4AAF-98B3-E7EA0E17E8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452B9490-4073-4A7E-A8EB-AB378608446A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="70320" yWindow="1770" windowWidth="17280" windowHeight="8910" firstSheet="8" activeTab="10" xr2:uid="{E053B55C-EE4D-4A44-BED7-23BE03F9DD4F}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="9" xr2:uid="{E053B55C-EE4D-4A44-BED7-23BE03F9DD4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Persona" sheetId="4" r:id="rId1"/>
@@ -1354,7 +1354,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="169" formatCode="0_);\(0\)"/>
+    <numFmt numFmtId="165" formatCode="0_);\(0\)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1455,7 +1455,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2972,7 +2972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E9E211F-CA5C-428B-BD4B-D943D5F61C98}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -3263,7 +3263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EEC2813-E6D4-4189-B69D-83FF52F8F158}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>